<commit_message>
Fixed issues with finding correct addresses
</commit_message>
<xml_diff>
--- a/Gen VI.xlsx
+++ b/Gen VI.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abzb1\Dropbox\Programs\Level-Recurver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01E29A24-F9B3-4EA5-B6A4-AB09BBCA38F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2FBACD1-C6E3-4E96-8465-6750136CFA59}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="13800" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="413" windowWidth="25787" windowHeight="13987" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="trdata 038" sheetId="1" r:id="rId1"/>
@@ -803,8 +803,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -1132,7 +1132,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
@@ -1161,7 +1161,7 @@
         <v>45</v>
       </c>
       <c r="B3" t="str">
-        <f t="shared" ref="B3:B17" si="0">_xlfn.CONCAT(B2,A3,",")</f>
+        <f t="shared" ref="B3:B16" si="0">_xlfn.CONCAT(B2,A3,",")</f>
         <v>[4,41,45,</v>
       </c>
     </row>

</xml_diff>